<commit_message>
Updated rv32 bitmanip vplan to v1.0.0
Signed-off-by: Henrik Fegran <Henrik.Fegran@silabs.com>
</commit_message>
<xml_diff>
--- a/docs/VerifPlans/ISA/RV32/Simulation/RV32B_Extension_Instructions.xlsx
+++ b/docs/VerifPlans/ISA/RV32/Simulation/RV32B_Extension_Instructions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\OneDrive\Desktop\New Vplan Updates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hefegran\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BA96CC7-85E7-4A0C-BF00-8098D5C6204B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA1FD69A-6928-41BB-AAC1-05E62F9C0510}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="58275" yWindow="2070" windowWidth="21195" windowHeight="14475" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="18240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RV32B" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="149">
   <si>
     <t>Requirement Location</t>
   </si>
@@ -125,17 +125,7 @@
 All possible register combinations where rs1 == rd are used</t>
   </si>
   <si>
-    <t>RISC-V Bitmanip Extension Version 0.93</t>
-  </si>
-  <si>
-    <t>RVB</t>
-  </si>
-  <si>
     <t>Extercise Bitmanip extensions freely intermixed with other instructions</t>
-  </si>
-  <si>
-    <t>RISC-V Bitmanip Extension Version 0.93
-Section 2.10</t>
   </si>
   <si>
     <t>Zba Extension</t>
@@ -188,10 +178,6 @@
     <t>Zbb Externsion</t>
   </si>
   <si>
-    <t>RISC-V Bitmanip Extension Version 0.93
-Section 2.1.1</t>
-  </si>
-  <si>
     <t>CLZ</t>
   </si>
   <si>
@@ -231,10 +217,6 @@
 Counts the numbrer of 1 bits in the value rs and places that value in rd</t>
   </si>
   <si>
-    <t>RISC-V Bitmanip Extension Version 0.93
-Section 2.1.2</t>
-  </si>
-  <si>
     <t>MIN</t>
   </si>
   <si>
@@ -267,10 +249,6 @@
 Compare rs1 and rs2 using an unsigned comparator and place the greater value in rd</t>
   </si>
   <si>
-    <t>RISC-V Bitmanip Extension Version 0.93
-Section 2.1.5</t>
-  </si>
-  <si>
     <t>SEXT.B</t>
   </si>
   <si>
@@ -290,10 +268,6 @@
     <t>sext.h rd, rs
 rd = { {16{rs[15]}}, rs[15:0] }
 Convert the signed 16-bit number in rs[15:0] to a 32-bit number by sign-extending and place the number into rd</t>
-  </si>
-  <si>
-    <t>RISC-V Bitmanip Extension Version 0.93
-Section 2.1.6</t>
   </si>
   <si>
     <t>ANDN</t>
@@ -324,10 +298,6 @@
 Bit-wise OR rs1 with the bit-wise inverted rs2 value and place into rd</t>
   </si>
   <si>
-    <t>RISC-V Bitmanip Extension Version 0.93
-Section 2.1.3</t>
-  </si>
-  <si>
     <t>XNOR</t>
   </si>
   <si>
@@ -373,10 +343,6 @@
 rd = rs1 rotate_right rs2
 rs1 is shifted left by the number of bits in rs2.
 Any bits shifted out of the MSB are shifted into the LSB of the output value</t>
-  </si>
-  <si>
-    <t>RISC-V Bitmanip Extension Version 0.93
-Section 2.2.1</t>
   </si>
   <si>
     <t>REV8</t>
@@ -403,22 +369,10 @@
 For each byte of rs, if the value is zero, the corresponding output value byte is set to all ones, other the byte is set to all zeroes</t>
   </si>
   <si>
-    <t>RISC-V Bitmanip Extension Version 0.93
-Section 2.3</t>
-  </si>
-  <si>
-    <t>RISC-V Bitmanip Extension Version 0.93
-Section 2.2.2</t>
-  </si>
-  <si>
     <t>Zbc Extension</t>
   </si>
   <si>
     <t>CLMUL</t>
-  </si>
-  <si>
-    <t>RISC-V Bitmanip Extension Version 0.93
-Section 2.6</t>
   </si>
   <si>
     <t xml:space="preserve">clmul rd, rs1, rs2
@@ -442,18 +396,12 @@
 </t>
   </si>
   <si>
-    <t>CULMULR</t>
-  </si>
-  <si>
     <t xml:space="preserve">clmulh rd, rs1, rs2
 rd = carry_less_product(rs1, rs2) &gt;&gt; 33
 The upper-half of the carry-less product of rs1 and rs2 is placed in rd
 </t>
   </si>
   <si>
-    <t>Zbe Extension</t>
-  </si>
-  <si>
     <t>BSET</t>
   </si>
   <si>
@@ -468,10 +416,6 @@
 All bit position values of [0,31] are used</t>
   </si>
   <si>
-    <t>RISC-V Bitmanip Extension Version 0.93
-Section 2.1.7</t>
-  </si>
-  <si>
     <t>BSETI</t>
   </si>
   <si>
@@ -532,13 +476,161 @@
     <t>binvi rd, rs1, imm
 rd = (rs1 &gt;&gt; imm) &amp; 0x1
 The bit position defined by the immediate value is extracted from rs1 and placed in the LSB of rd</t>
+  </si>
+  <si>
+    <t>CLMULR</t>
+  </si>
+  <si>
+    <t>RV Zb*</t>
+  </si>
+  <si>
+    <t>RISC-V Bitmanip Extension Version 1.0.0.38-g865e7a7</t>
+  </si>
+  <si>
+    <t>RISC-V Bitmanip Extension Version 1.0.0.38-g865e7a7
+Section 2.35</t>
+  </si>
+  <si>
+    <t>RISC-V Bitmanip Extension Version 1.0.0.38-g865e7a7
+Section 2.37</t>
+  </si>
+  <si>
+    <t>RISC-V Bitmanip Extension Version 1.0.0.38-g865e7a7
+Section 2.39</t>
+  </si>
+  <si>
+    <t>RISC-V Bitmanip Extension Version 1.0.0.38-g865e7a7
+Section 2.14</t>
+  </si>
+  <si>
+    <t>RISC-V Bitmanip Extension Version 1.0.0.38-g865e7a7
+Section 2.18</t>
+  </si>
+  <si>
+    <t>RISC-V Bitmanip Extension Version 1.0.0.38-g865e7a7
+Section 2.16</t>
+  </si>
+  <si>
+    <t>RISC-V Bitmanip Extension Version 1.0.0.38-g865e7a7
+Section 2.22</t>
+  </si>
+  <si>
+    <t>RISC-V Bitmanip Extension Version 1.0.0.38-g865e7a7
+Section 2.23</t>
+  </si>
+  <si>
+    <t>RISC-V Bitmanip Extension Version 1.0.0.38-g865e7a7
+Section 2.20</t>
+  </si>
+  <si>
+    <t>RISC-V Bitmanip Extension Version 1.0.0.38-g865e7a7
+Section 2.21</t>
+  </si>
+  <si>
+    <t>RISC-V Bitmanip Extension Version 1.0.0.38-g865e7a7
+Section 2.33</t>
+  </si>
+  <si>
+    <t>RISC-V Bitmanip Extension Version 1.0.0.38-g865e7a7
+Section 2.34</t>
+  </si>
+  <si>
+    <t>RISC-V Bitmanip Extension Version 1.0.0.38-g865e7a7
+Section 2.2</t>
+  </si>
+  <si>
+    <t>RISC-V Bitmanip Extension Version 1.0.0.38-g865e7a7
+Section 2.25</t>
+  </si>
+  <si>
+    <t>RISC-V Bitmanip Extension Version 1.0.0.38-g865e7a7
+Section 2.42</t>
+  </si>
+  <si>
+    <t>RISC-V Bitmanip Extension Version 1.0.0.38-g865e7a7
+Section 2.29</t>
+  </si>
+  <si>
+    <t>RISC-V Bitmanip Extension Version 1.0.0.38-g865e7a7
+Section 2.30</t>
+  </si>
+  <si>
+    <t>RISC-V Bitmanip Extension Version 1.0.0.38-g865e7a7
+Section 2.27</t>
+  </si>
+  <si>
+    <t>RISC-V Bitmanip Extension Version 1.0.0.38-g865e7a7
+Section 2.26</t>
+  </si>
+  <si>
+    <t>RISC-V Bitmanip Extension Version 1.0.0.38-g865e7a7
+Section 2.24</t>
+  </si>
+  <si>
+    <t>RISC-V Bitmanip Extension Version 1.0.0.38-g865e7a7
+Section 2.11</t>
+  </si>
+  <si>
+    <t>RISC-V Bitmanip Extension Version 1.0.0.38-g865e7a7
+Section 2.12</t>
+  </si>
+  <si>
+    <t>RISC-V Bitmanip Extension Version 1.0.0.38-g865e7a7
+Section 2.13</t>
+  </si>
+  <si>
+    <t>RISC-V Bitmanip Extension Version 1.0.0.38-g865e7a7
+Section 2.9</t>
+  </si>
+  <si>
+    <t>RISC-V Bitmanip Extension Version 1.0.0.38-g865e7a7
+Section 2.10</t>
+  </si>
+  <si>
+    <t>RISC-V Bitmanip Extension Version 1.0.0.38-g865e7a7
+Section 2.3</t>
+  </si>
+  <si>
+    <t>RISC-V Bitmanip Extension Version 1.0.0.38-g865e7a7
+Section 2.4</t>
+  </si>
+  <si>
+    <t>RISC-V Bitmanip Extension Version 1.0.0.38-g865e7a7
+Section 2.7</t>
+  </si>
+  <si>
+    <t>RISC-V Bitmanip Extension Version 1.0.0.38-g865e7a7
+Section 2.8</t>
+  </si>
+  <si>
+    <t>RISC-V Bitmanip Extension Version 1.0.0.38-g865e7a7
+Section 2.5</t>
+  </si>
+  <si>
+    <t>RISC-V Bitmanip Extension Version 1.0.0.38-g865e7a7
+Section 2.6</t>
+  </si>
+  <si>
+    <t>Zbs Extension</t>
+  </si>
+  <si>
+    <t>ZEXT.H</t>
+  </si>
+  <si>
+    <t>RISC-V Bitmanip Extension Version 1.0.0.38-g865e7a7
+Section 2.43</t>
+  </si>
+  <si>
+    <t>zext.h rd, rs
+rd = { {16{0}}, rs[15:0] }
+Convert the 16-bit number in rs[15:0] to a 32-bit number by zero-extending and place the number into rd</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -581,26 +673,6 @@
       <color rgb="FF000000"/>
       <name val="DejaVuSans"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="DejaVuSans"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -634,7 +706,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -687,34 +759,25 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1100,11 +1163,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMJ97"/>
+  <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E54" sqref="E54"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17" defaultRowHeight="15"/>
@@ -1153,17 +1216,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="10" customFormat="1" ht="57">
+    <row r="2" spans="1:10" s="10" customFormat="1" ht="90">
       <c r="A2" s="6" t="s">
-        <v>31</v>
+        <v>113</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>32</v>
+        <v>112</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
       <c r="E2" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>17</v>
@@ -1177,21 +1240,21 @@
       <c r="I2" s="9"/>
       <c r="J2" s="6"/>
     </row>
-    <row r="3" spans="1:10" s="10" customFormat="1" ht="99.75">
-      <c r="A3" s="25" t="s">
+    <row r="3" spans="1:10" s="10" customFormat="1" ht="135">
+      <c r="A3" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="E3" s="8" t="s">
         <v>35</v>
-      </c>
-      <c r="C3" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="D3" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>38</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>17</v>
@@ -1205,13 +1268,13 @@
       <c r="I3" s="6"/>
       <c r="J3" s="11"/>
     </row>
-    <row r="4" spans="1:10" s="10" customFormat="1" ht="85.5">
-      <c r="A4" s="25"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="28"/>
+    <row r="4" spans="1:10" s="10" customFormat="1" ht="90">
+      <c r="A4" s="22"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="25"/>
       <c r="D4" s="23"/>
       <c r="E4" s="17" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>17</v>
@@ -1225,13 +1288,13 @@
       <c r="I4" s="9"/>
       <c r="J4" s="12"/>
     </row>
-    <row r="5" spans="1:10" s="10" customFormat="1" ht="57">
-      <c r="A5" s="25"/>
-      <c r="B5" s="24"/>
-      <c r="C5" s="28"/>
+    <row r="5" spans="1:10" s="10" customFormat="1" ht="60">
+      <c r="A5" s="22"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="25"/>
       <c r="D5" s="23"/>
       <c r="E5" s="8" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F5" s="9" t="s">
         <v>17</v>
@@ -1245,17 +1308,19 @@
       <c r="I5" s="9"/>
       <c r="J5" s="12"/>
     </row>
-    <row r="6" spans="1:10" s="10" customFormat="1" ht="99.75">
-      <c r="A6" s="25"/>
-      <c r="B6" s="24"/>
-      <c r="C6" s="28" t="s">
+    <row r="6" spans="1:10" s="10" customFormat="1" ht="135">
+      <c r="A6" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="B6" s="22"/>
+      <c r="C6" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="D6" s="23" t="s">
-        <v>44</v>
-      </c>
       <c r="E6" s="17" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F6" s="9" t="s">
         <v>17</v>
@@ -1269,13 +1334,13 @@
       <c r="I6" s="6"/>
       <c r="J6" s="11"/>
     </row>
-    <row r="7" spans="1:10" s="10" customFormat="1" ht="85.5">
-      <c r="A7" s="25"/>
-      <c r="B7" s="24"/>
-      <c r="C7" s="28"/>
+    <row r="7" spans="1:10" s="10" customFormat="1" ht="90">
+      <c r="A7" s="22"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="25"/>
       <c r="D7" s="23"/>
       <c r="E7" s="17" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F7" s="9" t="s">
         <v>17</v>
@@ -1289,13 +1354,13 @@
       <c r="I7" s="9"/>
       <c r="J7" s="12"/>
     </row>
-    <row r="8" spans="1:10" s="10" customFormat="1" ht="57">
-      <c r="A8" s="25"/>
-      <c r="B8" s="24"/>
-      <c r="C8" s="28"/>
+    <row r="8" spans="1:10" s="10" customFormat="1" ht="60">
+      <c r="A8" s="22"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="25"/>
       <c r="D8" s="23"/>
       <c r="E8" s="17" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F8" s="9" t="s">
         <v>17</v>
@@ -1309,17 +1374,19 @@
       <c r="I8" s="9"/>
       <c r="J8" s="12"/>
     </row>
-    <row r="9" spans="1:10" s="10" customFormat="1" ht="99.75">
-      <c r="A9" s="25"/>
-      <c r="B9" s="24"/>
-      <c r="C9" s="28" t="s">
-        <v>42</v>
+    <row r="9" spans="1:10" s="10" customFormat="1" ht="135">
+      <c r="A9" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="B9" s="22"/>
+      <c r="C9" s="25" t="s">
+        <v>39</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F9" s="9" t="s">
         <v>17</v>
@@ -1333,13 +1400,13 @@
       <c r="I9" s="9"/>
       <c r="J9" s="12"/>
     </row>
-    <row r="10" spans="1:10" s="10" customFormat="1" ht="85.5">
-      <c r="A10" s="25"/>
-      <c r="B10" s="24"/>
-      <c r="C10" s="28"/>
+    <row r="10" spans="1:10" s="10" customFormat="1" ht="90">
+      <c r="A10" s="22"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="25"/>
       <c r="D10" s="23"/>
       <c r="E10" s="17" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F10" s="9" t="s">
         <v>17</v>
@@ -1353,13 +1420,13 @@
       <c r="I10" s="9"/>
       <c r="J10" s="12"/>
     </row>
-    <row r="11" spans="1:10" s="10" customFormat="1" ht="57">
-      <c r="A11" s="25"/>
-      <c r="B11" s="24"/>
-      <c r="C11" s="28"/>
+    <row r="11" spans="1:10" s="10" customFormat="1" ht="60">
+      <c r="A11" s="22"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="25"/>
       <c r="D11" s="23"/>
       <c r="E11" s="17" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F11" s="9" t="s">
         <v>17</v>
@@ -1373,21 +1440,21 @@
       <c r="I11" s="9"/>
       <c r="J11" s="12"/>
     </row>
-    <row r="12" spans="1:10" s="10" customFormat="1" ht="71.25">
-      <c r="A12" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="B12" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="C12" s="28" t="s">
-        <v>47</v>
+    <row r="12" spans="1:10" s="10" customFormat="1" ht="90" customHeight="1">
+      <c r="A12" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="B12" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="25" t="s">
+        <v>43</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F12" s="9" t="s">
         <v>17</v>
@@ -1401,13 +1468,13 @@
       <c r="I12" s="7"/>
       <c r="J12" s="11"/>
     </row>
-    <row r="13" spans="1:10" s="10" customFormat="1" ht="57">
-      <c r="A13" s="25"/>
-      <c r="B13" s="24"/>
-      <c r="C13" s="28"/>
+    <row r="13" spans="1:10" s="10" customFormat="1" ht="60">
+      <c r="A13" s="22"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="25"/>
       <c r="D13" s="23"/>
       <c r="E13" s="17" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F13" s="9" t="s">
         <v>17</v>
@@ -1421,13 +1488,13 @@
       <c r="I13" s="17"/>
       <c r="J13" s="12"/>
     </row>
-    <row r="14" spans="1:10" s="10" customFormat="1" ht="42.75">
-      <c r="A14" s="25"/>
-      <c r="B14" s="24"/>
-      <c r="C14" s="28"/>
+    <row r="14" spans="1:10" s="10" customFormat="1" ht="45">
+      <c r="A14" s="22"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="25"/>
       <c r="D14" s="23"/>
       <c r="E14" s="17" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F14" s="9" t="s">
         <v>17</v>
@@ -1442,16 +1509,18 @@
       <c r="J14" s="9"/>
     </row>
     <row r="15" spans="1:10" s="10" customFormat="1" ht="95.25" customHeight="1">
-      <c r="A15" s="25"/>
-      <c r="B15" s="24"/>
-      <c r="C15" s="29" t="s">
-        <v>51</v>
+      <c r="A15" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="B15" s="22"/>
+      <c r="C15" s="25" t="s">
+        <v>47</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E15" s="17" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F15" s="9" t="s">
         <v>17</v>
@@ -1465,13 +1534,13 @@
       <c r="I15" s="7"/>
       <c r="J15" s="11"/>
     </row>
-    <row r="16" spans="1:10" s="10" customFormat="1" ht="57">
-      <c r="A16" s="25"/>
-      <c r="B16" s="24"/>
-      <c r="C16" s="29"/>
+    <row r="16" spans="1:10" s="10" customFormat="1" ht="60">
+      <c r="A16" s="22"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="25"/>
       <c r="D16" s="23"/>
       <c r="E16" s="17" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F16" s="9" t="s">
         <v>17</v>
@@ -1485,13 +1554,13 @@
       <c r="I16" s="16"/>
       <c r="J16" s="12"/>
     </row>
-    <row r="17" spans="1:10" s="10" customFormat="1" ht="42.75">
-      <c r="A17" s="25"/>
-      <c r="B17" s="24"/>
-      <c r="C17" s="29"/>
+    <row r="17" spans="1:10" s="10" customFormat="1" ht="45">
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="25"/>
       <c r="D17" s="23"/>
       <c r="E17" s="17" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F17" s="9" t="s">
         <v>17</v>
@@ -1506,18 +1575,18 @@
       <c r="J17" s="12"/>
     </row>
     <row r="18" spans="1:10" s="10" customFormat="1" ht="58.5" customHeight="1">
-      <c r="A18" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="B18" s="24"/>
-      <c r="C18" s="29" t="s">
-        <v>52</v>
+      <c r="A18" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="B18" s="22"/>
+      <c r="C18" s="25" t="s">
+        <v>48</v>
       </c>
       <c r="D18" s="23" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E18" s="17" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F18" s="9" t="s">
         <v>17</v>
@@ -1531,13 +1600,13 @@
       <c r="I18" s="7"/>
       <c r="J18" s="11"/>
     </row>
-    <row r="19" spans="1:10" s="10" customFormat="1" ht="57">
-      <c r="A19" s="25"/>
-      <c r="B19" s="24"/>
-      <c r="C19" s="29"/>
+    <row r="19" spans="1:10" s="10" customFormat="1" ht="60">
+      <c r="A19" s="22"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="25"/>
       <c r="D19" s="23"/>
       <c r="E19" s="17" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F19" s="9" t="s">
         <v>17</v>
@@ -1551,13 +1620,13 @@
       <c r="I19" s="8"/>
       <c r="J19" s="12"/>
     </row>
-    <row r="20" spans="1:10" s="10" customFormat="1" ht="42.75">
-      <c r="A20" s="25"/>
-      <c r="B20" s="24"/>
-      <c r="C20" s="29"/>
+    <row r="20" spans="1:10" s="10" customFormat="1" ht="45">
+      <c r="A20" s="22"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="25"/>
       <c r="D20" s="23"/>
       <c r="E20" s="17" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F20" s="9" t="s">
         <v>17</v>
@@ -1572,18 +1641,18 @@
       <c r="J20" s="12"/>
     </row>
     <row r="21" spans="1:10" s="10" customFormat="1" ht="128.25" customHeight="1">
-      <c r="A21" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="B21" s="24"/>
-      <c r="C21" s="29" t="s">
-        <v>57</v>
+      <c r="A21" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="B21" s="22"/>
+      <c r="C21" s="25" t="s">
+        <v>52</v>
       </c>
       <c r="D21" s="23" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="E21" s="17" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F21" s="9" t="s">
         <v>17</v>
@@ -1597,13 +1666,13 @@
       <c r="I21" s="7"/>
       <c r="J21" s="11"/>
     </row>
-    <row r="22" spans="1:10" s="10" customFormat="1" ht="85.5">
-      <c r="A22" s="25"/>
-      <c r="B22" s="24"/>
-      <c r="C22" s="29"/>
+    <row r="22" spans="1:10" s="10" customFormat="1" ht="90">
+      <c r="A22" s="22"/>
+      <c r="B22" s="22"/>
+      <c r="C22" s="25"/>
       <c r="D22" s="23"/>
       <c r="E22" s="17" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F22" s="9" t="s">
         <v>17</v>
@@ -1617,13 +1686,13 @@
       <c r="I22" s="8"/>
       <c r="J22" s="12"/>
     </row>
-    <row r="23" spans="1:10" s="10" customFormat="1" ht="57">
-      <c r="A23" s="25"/>
-      <c r="B23" s="24"/>
-      <c r="C23" s="29"/>
+    <row r="23" spans="1:10" s="10" customFormat="1" ht="60">
+      <c r="A23" s="22"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="25"/>
       <c r="D23" s="23"/>
       <c r="E23" s="17" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F23" s="9" t="s">
         <v>17</v>
@@ -1638,16 +1707,18 @@
       <c r="J23" s="12"/>
     </row>
     <row r="24" spans="1:10" s="10" customFormat="1" ht="128.25" customHeight="1">
-      <c r="A24" s="25"/>
-      <c r="B24" s="24"/>
-      <c r="C24" s="29" t="s">
-        <v>59</v>
+      <c r="A24" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="B24" s="22"/>
+      <c r="C24" s="25" t="s">
+        <v>54</v>
       </c>
       <c r="D24" s="23" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E24" s="17" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F24" s="9" t="s">
         <v>17</v>
@@ -1661,13 +1732,13 @@
       <c r="I24" s="7"/>
       <c r="J24" s="11"/>
     </row>
-    <row r="25" spans="1:10" s="10" customFormat="1" ht="85.5">
-      <c r="A25" s="25"/>
-      <c r="B25" s="24"/>
-      <c r="C25" s="29"/>
+    <row r="25" spans="1:10" s="10" customFormat="1" ht="90">
+      <c r="A25" s="22"/>
+      <c r="B25" s="22"/>
+      <c r="C25" s="25"/>
       <c r="D25" s="23"/>
       <c r="E25" s="17" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F25" s="9" t="s">
         <v>17</v>
@@ -1681,13 +1752,13 @@
       <c r="I25" s="8"/>
       <c r="J25" s="12"/>
     </row>
-    <row r="26" spans="1:10" s="10" customFormat="1" ht="57">
-      <c r="A26" s="25"/>
-      <c r="B26" s="24"/>
-      <c r="C26" s="29"/>
+    <row r="26" spans="1:10" s="10" customFormat="1" ht="60">
+      <c r="A26" s="22"/>
+      <c r="B26" s="22"/>
+      <c r="C26" s="25"/>
       <c r="D26" s="23"/>
       <c r="E26" s="17" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F26" s="9" t="s">
         <v>17</v>
@@ -1702,16 +1773,18 @@
       <c r="J26" s="12"/>
     </row>
     <row r="27" spans="1:10" s="10" customFormat="1" ht="128.25" customHeight="1">
-      <c r="A27" s="25"/>
-      <c r="B27" s="24"/>
-      <c r="C27" s="29" t="s">
-        <v>61</v>
+      <c r="A27" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="B27" s="22"/>
+      <c r="C27" s="25" t="s">
+        <v>56</v>
       </c>
       <c r="D27" s="23" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E27" s="17" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F27" s="9" t="s">
         <v>17</v>
@@ -1725,13 +1798,13 @@
       <c r="I27" s="7"/>
       <c r="J27" s="11"/>
     </row>
-    <row r="28" spans="1:10" s="10" customFormat="1" ht="85.5">
-      <c r="A28" s="25"/>
-      <c r="B28" s="24"/>
-      <c r="C28" s="29"/>
+    <row r="28" spans="1:10" s="10" customFormat="1" ht="90">
+      <c r="A28" s="22"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="25"/>
       <c r="D28" s="23"/>
       <c r="E28" s="17" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F28" s="9" t="s">
         <v>17</v>
@@ -1745,13 +1818,13 @@
       <c r="I28" s="16"/>
       <c r="J28" s="12"/>
     </row>
-    <row r="29" spans="1:10" s="10" customFormat="1" ht="57">
-      <c r="A29" s="25"/>
-      <c r="B29" s="24"/>
-      <c r="C29" s="29"/>
+    <row r="29" spans="1:10" s="10" customFormat="1" ht="60">
+      <c r="A29" s="22"/>
+      <c r="B29" s="22"/>
+      <c r="C29" s="25"/>
       <c r="D29" s="23"/>
       <c r="E29" s="17" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F29" s="9" t="s">
         <v>17</v>
@@ -1766,16 +1839,18 @@
       <c r="J29" s="12"/>
     </row>
     <row r="30" spans="1:10" s="10" customFormat="1" ht="128.25" customHeight="1">
-      <c r="A30" s="25"/>
-      <c r="B30" s="24"/>
-      <c r="C30" s="29" t="s">
-        <v>62</v>
+      <c r="A30" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="B30" s="22"/>
+      <c r="C30" s="25" t="s">
+        <v>57</v>
       </c>
       <c r="D30" s="23" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E30" s="17" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F30" s="9" t="s">
         <v>17</v>
@@ -1789,13 +1864,13 @@
       <c r="I30" s="16"/>
       <c r="J30" s="12"/>
     </row>
-    <row r="31" spans="1:10" s="10" customFormat="1" ht="85.5">
-      <c r="A31" s="25"/>
-      <c r="B31" s="24"/>
-      <c r="C31" s="29"/>
+    <row r="31" spans="1:10" s="10" customFormat="1" ht="90">
+      <c r="A31" s="22"/>
+      <c r="B31" s="22"/>
+      <c r="C31" s="25"/>
       <c r="D31" s="23"/>
       <c r="E31" s="17" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F31" s="9" t="s">
         <v>17</v>
@@ -1809,13 +1884,13 @@
       <c r="I31" s="16"/>
       <c r="J31" s="12"/>
     </row>
-    <row r="32" spans="1:10" s="10" customFormat="1" ht="57">
-      <c r="A32" s="25"/>
-      <c r="B32" s="24"/>
-      <c r="C32" s="29"/>
+    <row r="32" spans="1:10" s="10" customFormat="1" ht="60">
+      <c r="A32" s="22"/>
+      <c r="B32" s="22"/>
+      <c r="C32" s="25"/>
       <c r="D32" s="23"/>
       <c r="E32" s="17" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F32" s="9" t="s">
         <v>17</v>
@@ -1829,19 +1904,19 @@
       <c r="I32" s="17"/>
       <c r="J32" s="12"/>
     </row>
-    <row r="33" spans="1:10" s="10" customFormat="1" ht="71.25">
-      <c r="A33" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="B33" s="24"/>
-      <c r="C33" s="29" t="s">
-        <v>66</v>
+    <row r="33" spans="1:10" s="10" customFormat="1" ht="90">
+      <c r="A33" s="22" t="s">
+        <v>124</v>
+      </c>
+      <c r="B33" s="22"/>
+      <c r="C33" s="25" t="s">
+        <v>60</v>
       </c>
       <c r="D33" s="23" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="E33" s="17" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F33" s="9" t="s">
         <v>17</v>
@@ -1855,13 +1930,13 @@
       <c r="I33" s="7"/>
       <c r="J33" s="11"/>
     </row>
-    <row r="34" spans="1:10" s="10" customFormat="1" ht="57">
-      <c r="A34" s="25"/>
-      <c r="B34" s="24"/>
-      <c r="C34" s="29"/>
+    <row r="34" spans="1:10" s="10" customFormat="1" ht="60">
+      <c r="A34" s="22"/>
+      <c r="B34" s="22"/>
+      <c r="C34" s="25"/>
       <c r="D34" s="23"/>
       <c r="E34" s="17" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F34" s="9" t="s">
         <v>17</v>
@@ -1875,13 +1950,13 @@
       <c r="I34" s="16"/>
       <c r="J34" s="12"/>
     </row>
-    <row r="35" spans="1:10" s="10" customFormat="1" ht="57">
-      <c r="A35" s="25"/>
-      <c r="B35" s="24"/>
-      <c r="C35" s="29"/>
+    <row r="35" spans="1:10" s="10" customFormat="1" ht="60">
+      <c r="A35" s="22"/>
+      <c r="B35" s="22"/>
+      <c r="C35" s="25"/>
       <c r="D35" s="23"/>
       <c r="E35" s="17" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="F35" s="9" t="s">
         <v>17</v>
@@ -1895,17 +1970,19 @@
       <c r="I35" s="16"/>
       <c r="J35" s="12"/>
     </row>
-    <row r="36" spans="1:10" s="10" customFormat="1" ht="71.25">
-      <c r="A36" s="25"/>
-      <c r="B36" s="24"/>
-      <c r="C36" s="29" t="s">
-        <v>69</v>
+    <row r="36" spans="1:10" s="10" customFormat="1" ht="90">
+      <c r="A36" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="B36" s="22"/>
+      <c r="C36" s="25" t="s">
+        <v>63</v>
       </c>
       <c r="D36" s="23" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E36" s="17" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F36" s="9" t="s">
         <v>17</v>
@@ -1919,13 +1996,13 @@
       <c r="I36" s="7"/>
       <c r="J36" s="11"/>
     </row>
-    <row r="37" spans="1:10" s="10" customFormat="1" ht="57">
-      <c r="A37" s="25"/>
-      <c r="B37" s="24"/>
-      <c r="C37" s="29"/>
+    <row r="37" spans="1:10" s="10" customFormat="1" ht="60">
+      <c r="A37" s="22"/>
+      <c r="B37" s="22"/>
+      <c r="C37" s="25"/>
       <c r="D37" s="23"/>
       <c r="E37" s="17" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F37" s="9" t="s">
         <v>17</v>
@@ -1939,13 +2016,13 @@
       <c r="I37" s="16"/>
       <c r="J37" s="12"/>
     </row>
-    <row r="38" spans="1:10" s="10" customFormat="1" ht="57">
-      <c r="A38" s="25"/>
-      <c r="B38" s="24"/>
-      <c r="C38" s="29"/>
+    <row r="38" spans="1:10" s="10" customFormat="1" ht="60">
+      <c r="A38" s="22"/>
+      <c r="B38" s="22"/>
+      <c r="C38" s="25"/>
       <c r="D38" s="23"/>
       <c r="E38" s="17" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="F38" s="9" t="s">
         <v>17</v>
@@ -1959,19 +2036,19 @@
       <c r="I38" s="16"/>
       <c r="J38" s="12"/>
     </row>
-    <row r="39" spans="1:10" s="10" customFormat="1" ht="99.75">
-      <c r="A39" s="25" t="s">
-        <v>78</v>
-      </c>
-      <c r="B39" s="24"/>
-      <c r="C39" s="26" t="s">
-        <v>72</v>
+    <row r="39" spans="1:10" s="10" customFormat="1" ht="135">
+      <c r="A39" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="B39" s="22"/>
+      <c r="C39" s="25" t="s">
+        <v>65</v>
       </c>
       <c r="D39" s="23" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="E39" s="17" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F39" s="9" t="s">
         <v>17</v>
@@ -1985,13 +2062,13 @@
       <c r="I39" s="17"/>
       <c r="J39" s="12"/>
     </row>
-    <row r="40" spans="1:10" s="10" customFormat="1" ht="85.5">
-      <c r="A40" s="25"/>
-      <c r="B40" s="24"/>
-      <c r="C40" s="26"/>
+    <row r="40" spans="1:10" s="10" customFormat="1" ht="90">
+      <c r="A40" s="22"/>
+      <c r="B40" s="22"/>
+      <c r="C40" s="25"/>
       <c r="D40" s="23"/>
       <c r="E40" s="17" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="F40" s="9" t="s">
         <v>17</v>
@@ -2005,13 +2082,13 @@
       <c r="I40" s="17"/>
       <c r="J40" s="12"/>
     </row>
-    <row r="41" spans="1:10" s="10" customFormat="1" ht="57">
-      <c r="A41" s="25"/>
-      <c r="B41" s="24"/>
-      <c r="C41" s="26"/>
+    <row r="41" spans="1:10" s="10" customFormat="1" ht="60">
+      <c r="A41" s="22"/>
+      <c r="B41" s="22"/>
+      <c r="C41" s="25"/>
       <c r="D41" s="23"/>
       <c r="E41" s="17" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="F41" s="9" t="s">
         <v>17</v>
@@ -2025,17 +2102,19 @@
       <c r="I41" s="17"/>
       <c r="J41" s="12"/>
     </row>
-    <row r="42" spans="1:10" s="10" customFormat="1" ht="99.75">
-      <c r="A42" s="25"/>
-      <c r="B42" s="24"/>
-      <c r="C42" s="26" t="s">
-        <v>76</v>
+    <row r="42" spans="1:10" s="10" customFormat="1" ht="135">
+      <c r="A42" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="B42" s="22"/>
+      <c r="C42" s="25" t="s">
+        <v>69</v>
       </c>
       <c r="D42" s="23" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="E42" s="17" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F42" s="9" t="s">
         <v>17</v>
@@ -2049,13 +2128,13 @@
       <c r="I42" s="17"/>
       <c r="J42" s="12"/>
     </row>
-    <row r="43" spans="1:10" s="10" customFormat="1" ht="85.5">
-      <c r="A43" s="25"/>
-      <c r="B43" s="24"/>
-      <c r="C43" s="26"/>
+    <row r="43" spans="1:10" s="10" customFormat="1" ht="90">
+      <c r="A43" s="22"/>
+      <c r="B43" s="22"/>
+      <c r="C43" s="25"/>
       <c r="D43" s="23"/>
       <c r="E43" s="17" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="F43" s="9" t="s">
         <v>17</v>
@@ -2069,13 +2148,13 @@
       <c r="I43" s="17"/>
       <c r="J43" s="12"/>
     </row>
-    <row r="44" spans="1:10" s="10" customFormat="1" ht="57">
-      <c r="A44" s="25"/>
-      <c r="B44" s="24"/>
-      <c r="C44" s="26"/>
+    <row r="44" spans="1:10" s="10" customFormat="1" ht="60">
+      <c r="A44" s="22"/>
+      <c r="B44" s="22"/>
+      <c r="C44" s="25"/>
       <c r="D44" s="23"/>
       <c r="E44" s="17" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="F44" s="9" t="s">
         <v>17</v>
@@ -2089,17 +2168,19 @@
       <c r="I44" s="17"/>
       <c r="J44" s="12"/>
     </row>
-    <row r="45" spans="1:10" s="10" customFormat="1" ht="99.75">
-      <c r="A45" s="25"/>
-      <c r="B45" s="24"/>
-      <c r="C45" s="26" t="s">
-        <v>79</v>
+    <row r="45" spans="1:10" s="10" customFormat="1" ht="135">
+      <c r="A45" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="B45" s="22"/>
+      <c r="C45" s="25" t="s">
+        <v>71</v>
       </c>
       <c r="D45" s="23" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="E45" s="17" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F45" s="9" t="s">
         <v>17</v>
@@ -2113,13 +2194,13 @@
       <c r="I45" s="17"/>
       <c r="J45" s="12"/>
     </row>
-    <row r="46" spans="1:10" s="10" customFormat="1" ht="85.5">
-      <c r="A46" s="25"/>
-      <c r="B46" s="24"/>
-      <c r="C46" s="26"/>
+    <row r="46" spans="1:10" s="10" customFormat="1" ht="90">
+      <c r="A46" s="22"/>
+      <c r="B46" s="22"/>
+      <c r="C46" s="25"/>
       <c r="D46" s="23"/>
       <c r="E46" s="17" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="F46" s="9" t="s">
         <v>17</v>
@@ -2133,13 +2214,13 @@
       <c r="I46" s="17"/>
       <c r="J46" s="12"/>
     </row>
-    <row r="47" spans="1:10" s="10" customFormat="1" ht="57">
-      <c r="A47" s="25"/>
-      <c r="B47" s="24"/>
-      <c r="C47" s="26"/>
+    <row r="47" spans="1:10" s="10" customFormat="1" ht="60">
+      <c r="A47" s="22"/>
+      <c r="B47" s="22"/>
+      <c r="C47" s="25"/>
       <c r="D47" s="23"/>
       <c r="E47" s="17" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="F47" s="9" t="s">
         <v>17</v>
@@ -2153,19 +2234,19 @@
       <c r="I47" s="17"/>
       <c r="J47" s="12"/>
     </row>
-    <row r="48" spans="1:10" s="10" customFormat="1" ht="99.75">
-      <c r="A48" s="25" t="s">
-        <v>89</v>
-      </c>
-      <c r="B48" s="24"/>
-      <c r="C48" s="26" t="s">
-        <v>81</v>
+    <row r="48" spans="1:10" s="10" customFormat="1" ht="135">
+      <c r="A48" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="B48" s="22"/>
+      <c r="C48" s="25" t="s">
+        <v>73</v>
       </c>
       <c r="D48" s="23" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="E48" s="17" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F48" s="9" t="s">
         <v>17</v>
@@ -2179,13 +2260,13 @@
       <c r="I48" s="17"/>
       <c r="J48" s="12"/>
     </row>
-    <row r="49" spans="1:10" s="10" customFormat="1" ht="71.25">
-      <c r="A49" s="25"/>
-      <c r="B49" s="24"/>
-      <c r="C49" s="26"/>
+    <row r="49" spans="1:10" s="10" customFormat="1" ht="75">
+      <c r="A49" s="22"/>
+      <c r="B49" s="22"/>
+      <c r="C49" s="25"/>
       <c r="D49" s="23"/>
       <c r="E49" s="17" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="F49" s="9" t="s">
         <v>17</v>
@@ -2199,13 +2280,13 @@
       <c r="I49" s="17"/>
       <c r="J49" s="12"/>
     </row>
-    <row r="50" spans="1:10" s="10" customFormat="1" ht="57">
-      <c r="A50" s="25"/>
-      <c r="B50" s="24"/>
-      <c r="C50" s="26"/>
+    <row r="50" spans="1:10" s="10" customFormat="1" ht="60">
+      <c r="A50" s="22"/>
+      <c r="B50" s="22"/>
+      <c r="C50" s="25"/>
       <c r="D50" s="23"/>
       <c r="E50" s="17" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="F50" s="9" t="s">
         <v>17</v>
@@ -2219,14 +2300,16 @@
       <c r="I50" s="17"/>
       <c r="J50" s="12"/>
     </row>
-    <row r="51" spans="1:10" s="10" customFormat="1" ht="71.25">
-      <c r="A51" s="25"/>
-      <c r="B51" s="24"/>
-      <c r="C51" s="26" t="s">
-        <v>84</v>
+    <row r="51" spans="1:10" s="10" customFormat="1" ht="90">
+      <c r="A51" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="B51" s="22"/>
+      <c r="C51" s="25" t="s">
+        <v>76</v>
       </c>
       <c r="D51" s="23" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E51" s="17" t="s">
         <v>30</v>
@@ -2243,13 +2326,13 @@
       <c r="I51" s="17"/>
       <c r="J51" s="12"/>
     </row>
-    <row r="52" spans="1:10" s="10" customFormat="1" ht="71.25">
-      <c r="A52" s="25"/>
-      <c r="B52" s="24"/>
-      <c r="C52" s="26"/>
+    <row r="52" spans="1:10" s="10" customFormat="1" ht="75">
+      <c r="A52" s="22"/>
+      <c r="B52" s="22"/>
+      <c r="C52" s="25"/>
       <c r="D52" s="23"/>
       <c r="E52" s="17" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="F52" s="9" t="s">
         <v>17</v>
@@ -2263,13 +2346,13 @@
       <c r="I52" s="17"/>
       <c r="J52" s="12"/>
     </row>
-    <row r="53" spans="1:10" s="10" customFormat="1" ht="57">
-      <c r="A53" s="25"/>
-      <c r="B53" s="24"/>
-      <c r="C53" s="26"/>
+    <row r="53" spans="1:10" s="10" customFormat="1" ht="60">
+      <c r="A53" s="22"/>
+      <c r="B53" s="22"/>
+      <c r="C53" s="25"/>
       <c r="D53" s="23"/>
       <c r="E53" s="17" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="F53" s="9" t="s">
         <v>17</v>
@@ -2283,17 +2366,19 @@
       <c r="I53" s="17"/>
       <c r="J53" s="12"/>
     </row>
-    <row r="54" spans="1:10" s="10" customFormat="1" ht="99.75">
-      <c r="A54" s="25"/>
-      <c r="B54" s="24"/>
-      <c r="C54" s="26" t="s">
-        <v>87</v>
+    <row r="54" spans="1:10" s="10" customFormat="1" ht="135">
+      <c r="A54" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="B54" s="22"/>
+      <c r="C54" s="25" t="s">
+        <v>79</v>
       </c>
       <c r="D54" s="23" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="E54" s="17" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F54" s="9" t="s">
         <v>17</v>
@@ -2307,13 +2392,13 @@
       <c r="I54" s="17"/>
       <c r="J54" s="12"/>
     </row>
-    <row r="55" spans="1:10" s="10" customFormat="1" ht="71.25">
-      <c r="A55" s="25"/>
-      <c r="B55" s="24"/>
-      <c r="C55" s="26"/>
+    <row r="55" spans="1:10" s="10" customFormat="1" ht="75">
+      <c r="A55" s="22"/>
+      <c r="B55" s="22"/>
+      <c r="C55" s="25"/>
       <c r="D55" s="23"/>
       <c r="E55" s="17" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="F55" s="9" t="s">
         <v>17</v>
@@ -2327,13 +2412,13 @@
       <c r="I55" s="17"/>
       <c r="J55" s="12"/>
     </row>
-    <row r="56" spans="1:10" s="10" customFormat="1" ht="57">
-      <c r="A56" s="25"/>
-      <c r="B56" s="24"/>
-      <c r="C56" s="26"/>
+    <row r="56" spans="1:10" s="10" customFormat="1" ht="60">
+      <c r="A56" s="22"/>
+      <c r="B56" s="22"/>
+      <c r="C56" s="25"/>
       <c r="D56" s="23"/>
       <c r="E56" s="17" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="F56" s="9" t="s">
         <v>17</v>
@@ -2347,19 +2432,19 @@
       <c r="I56" s="17"/>
       <c r="J56" s="12"/>
     </row>
-    <row r="57" spans="1:10" s="10" customFormat="1" ht="71.25">
-      <c r="A57" s="25" t="s">
-        <v>96</v>
-      </c>
-      <c r="B57" s="24"/>
-      <c r="C57" s="26" t="s">
-        <v>90</v>
+    <row r="57" spans="1:10" s="10" customFormat="1" ht="90">
+      <c r="A57" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="B57" s="22"/>
+      <c r="C57" s="25" t="s">
+        <v>81</v>
       </c>
       <c r="D57" s="23" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="E57" s="17" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F57" s="9" t="s">
         <v>17</v>
@@ -2373,13 +2458,13 @@
       <c r="I57" s="17"/>
       <c r="J57" s="12"/>
     </row>
-    <row r="58" spans="1:10" s="10" customFormat="1" ht="57">
-      <c r="A58" s="25"/>
-      <c r="B58" s="24"/>
-      <c r="C58" s="26"/>
+    <row r="58" spans="1:10" s="10" customFormat="1" ht="60">
+      <c r="A58" s="22"/>
+      <c r="B58" s="22"/>
+      <c r="C58" s="25"/>
       <c r="D58" s="23"/>
       <c r="E58" s="17" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="F58" s="9" t="s">
         <v>17</v>
@@ -2393,10 +2478,10 @@
       <c r="I58" s="17"/>
       <c r="J58" s="12"/>
     </row>
-    <row r="59" spans="1:10" s="10" customFormat="1" ht="42.75">
-      <c r="A59" s="25"/>
-      <c r="B59" s="24"/>
-      <c r="C59" s="26"/>
+    <row r="59" spans="1:10" s="10" customFormat="1" ht="45">
+      <c r="A59" s="22"/>
+      <c r="B59" s="22"/>
+      <c r="C59" s="25"/>
       <c r="D59" s="23"/>
       <c r="E59" s="17" t="s">
         <v>29</v>
@@ -2414,18 +2499,18 @@
       <c r="J59" s="12"/>
     </row>
     <row r="60" spans="1:10" s="10" customFormat="1" ht="114" customHeight="1">
-      <c r="A60" s="25" t="s">
-        <v>95</v>
-      </c>
-      <c r="B60" s="24"/>
-      <c r="C60" s="26" t="s">
-        <v>93</v>
+      <c r="A60" s="22" t="s">
+        <v>133</v>
+      </c>
+      <c r="B60" s="22"/>
+      <c r="C60" s="25" t="s">
+        <v>84</v>
       </c>
       <c r="D60" s="23" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="E60" s="17" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F60" s="9" t="s">
         <v>17</v>
@@ -2439,13 +2524,13 @@
       <c r="I60" s="17"/>
       <c r="J60" s="12"/>
     </row>
-    <row r="61" spans="1:10" s="10" customFormat="1" ht="57">
-      <c r="A61" s="25"/>
-      <c r="B61" s="24"/>
-      <c r="C61" s="26"/>
+    <row r="61" spans="1:10" s="10" customFormat="1" ht="60">
+      <c r="A61" s="22"/>
+      <c r="B61" s="22"/>
+      <c r="C61" s="25"/>
       <c r="D61" s="23"/>
       <c r="E61" s="17" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="F61" s="9" t="s">
         <v>17</v>
@@ -2459,10 +2544,10 @@
       <c r="I61" s="17"/>
       <c r="J61" s="12"/>
     </row>
-    <row r="62" spans="1:10" s="10" customFormat="1" ht="42.75">
-      <c r="A62" s="25"/>
-      <c r="B62" s="24"/>
-      <c r="C62" s="26"/>
+    <row r="62" spans="1:10" s="10" customFormat="1" ht="45">
+      <c r="A62" s="22"/>
+      <c r="B62" s="22"/>
+      <c r="C62" s="25"/>
       <c r="D62" s="23"/>
       <c r="E62" s="17" t="s">
         <v>29</v>
@@ -2479,21 +2564,19 @@
       <c r="I62" s="17"/>
       <c r="J62" s="12"/>
     </row>
-    <row r="63" spans="1:10" s="10" customFormat="1" ht="99.75">
-      <c r="A63" s="25" t="s">
-        <v>99</v>
-      </c>
-      <c r="B63" s="24" t="s">
-        <v>97</v>
-      </c>
+    <row r="63" spans="1:10" s="10" customFormat="1" ht="107.25" customHeight="1">
+      <c r="A63" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="B63" s="22"/>
       <c r="C63" s="26" t="s">
-        <v>98</v>
+        <v>146</v>
       </c>
       <c r="D63" s="23" t="s">
-        <v>100</v>
+        <v>148</v>
       </c>
       <c r="E63" s="17" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="F63" s="9" t="s">
         <v>17</v>
@@ -2507,13 +2590,13 @@
       <c r="I63" s="17"/>
       <c r="J63" s="12"/>
     </row>
-    <row r="64" spans="1:10" s="10" customFormat="1" ht="71.25">
-      <c r="A64" s="25"/>
-      <c r="B64" s="24"/>
+    <row r="64" spans="1:10" s="10" customFormat="1" ht="81.75" customHeight="1">
+      <c r="A64" s="22"/>
+      <c r="B64" s="22"/>
       <c r="C64" s="26"/>
       <c r="D64" s="23"/>
       <c r="E64" s="17" t="s">
-        <v>101</v>
+        <v>45</v>
       </c>
       <c r="F64" s="9" t="s">
         <v>17</v>
@@ -2527,13 +2610,13 @@
       <c r="I64" s="17"/>
       <c r="J64" s="12"/>
     </row>
-    <row r="65" spans="1:10" s="10" customFormat="1" ht="57">
-      <c r="A65" s="25"/>
-      <c r="B65" s="24"/>
+    <row r="65" spans="1:10" s="10" customFormat="1" ht="77.25" customHeight="1">
+      <c r="A65" s="22"/>
+      <c r="B65" s="22"/>
       <c r="C65" s="26"/>
       <c r="D65" s="23"/>
       <c r="E65" s="17" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="F65" s="9" t="s">
         <v>17</v>
@@ -2547,17 +2630,21 @@
       <c r="I65" s="17"/>
       <c r="J65" s="12"/>
     </row>
-    <row r="66" spans="1:10" s="10" customFormat="1" ht="99.75">
-      <c r="A66" s="25"/>
-      <c r="B66" s="24"/>
-      <c r="C66" s="26" t="s">
-        <v>102</v>
+    <row r="66" spans="1:10" s="10" customFormat="1" ht="135">
+      <c r="A66" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="B66" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="C66" s="25" t="s">
+        <v>87</v>
       </c>
       <c r="D66" s="23" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="E66" s="17" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F66" s="9" t="s">
         <v>17</v>
@@ -2571,13 +2658,13 @@
       <c r="I66" s="17"/>
       <c r="J66" s="12"/>
     </row>
-    <row r="67" spans="1:10" s="10" customFormat="1" ht="71.25">
-      <c r="A67" s="25"/>
-      <c r="B67" s="24"/>
-      <c r="C67" s="26"/>
+    <row r="67" spans="1:10" s="10" customFormat="1" ht="75">
+      <c r="A67" s="21"/>
+      <c r="B67" s="22"/>
+      <c r="C67" s="25"/>
       <c r="D67" s="23"/>
       <c r="E67" s="17" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="F67" s="9" t="s">
         <v>17</v>
@@ -2591,13 +2678,13 @@
       <c r="I67" s="17"/>
       <c r="J67" s="12"/>
     </row>
-    <row r="68" spans="1:10" s="10" customFormat="1" ht="57">
-      <c r="A68" s="25"/>
-      <c r="B68" s="24"/>
-      <c r="C68" s="26"/>
+    <row r="68" spans="1:10" s="10" customFormat="1" ht="60">
+      <c r="A68" s="21"/>
+      <c r="B68" s="22"/>
+      <c r="C68" s="25"/>
       <c r="D68" s="23"/>
       <c r="E68" s="17" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="F68" s="9" t="s">
         <v>17</v>
@@ -2611,17 +2698,19 @@
       <c r="I68" s="17"/>
       <c r="J68" s="12"/>
     </row>
-    <row r="69" spans="1:10" s="10" customFormat="1" ht="99.75">
-      <c r="A69" s="25"/>
-      <c r="B69" s="24"/>
-      <c r="C69" s="26" t="s">
-        <v>104</v>
+    <row r="69" spans="1:10" s="10" customFormat="1" ht="135">
+      <c r="A69" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="B69" s="22"/>
+      <c r="C69" s="25" t="s">
+        <v>90</v>
       </c>
       <c r="D69" s="23" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="E69" s="17" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F69" s="9" t="s">
         <v>17</v>
@@ -2635,13 +2724,13 @@
       <c r="I69" s="17"/>
       <c r="J69" s="12"/>
     </row>
-    <row r="70" spans="1:10" s="10" customFormat="1" ht="71.25">
-      <c r="A70" s="25"/>
-      <c r="B70" s="24"/>
-      <c r="C70" s="26"/>
+    <row r="70" spans="1:10" s="10" customFormat="1" ht="75">
+      <c r="A70" s="21"/>
+      <c r="B70" s="22"/>
+      <c r="C70" s="25"/>
       <c r="D70" s="23"/>
       <c r="E70" s="17" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="F70" s="9" t="s">
         <v>17</v>
@@ -2655,13 +2744,13 @@
       <c r="I70" s="17"/>
       <c r="J70" s="12"/>
     </row>
-    <row r="71" spans="1:10" s="10" customFormat="1" ht="57">
-      <c r="A71" s="25"/>
-      <c r="B71" s="24"/>
-      <c r="C71" s="26"/>
+    <row r="71" spans="1:10" s="10" customFormat="1" ht="60">
+      <c r="A71" s="21"/>
+      <c r="B71" s="22"/>
+      <c r="C71" s="25"/>
       <c r="D71" s="23"/>
       <c r="E71" s="17" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="F71" s="9" t="s">
         <v>17</v>
@@ -2675,21 +2764,19 @@
       <c r="I71" s="17"/>
       <c r="J71" s="12"/>
     </row>
-    <row r="72" spans="1:10" s="10" customFormat="1" ht="99.75">
-      <c r="A72" s="25" t="s">
-        <v>110</v>
-      </c>
-      <c r="B72" s="24" t="s">
-        <v>106</v>
-      </c>
-      <c r="C72" s="20" t="s">
-        <v>107</v>
+    <row r="72" spans="1:10" s="10" customFormat="1" ht="135">
+      <c r="A72" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="B72" s="22"/>
+      <c r="C72" s="25" t="s">
+        <v>111</v>
       </c>
       <c r="D72" s="23" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="E72" s="17" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F72" s="9" t="s">
         <v>17</v>
@@ -2703,13 +2790,13 @@
       <c r="I72" s="17"/>
       <c r="J72" s="12"/>
     </row>
-    <row r="73" spans="1:10" s="10" customFormat="1" ht="71.25">
-      <c r="A73" s="25"/>
-      <c r="B73" s="24"/>
-      <c r="C73" s="20"/>
+    <row r="73" spans="1:10" s="10" customFormat="1" ht="75">
+      <c r="A73" s="21"/>
+      <c r="B73" s="22"/>
+      <c r="C73" s="25"/>
       <c r="D73" s="23"/>
       <c r="E73" s="17" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="F73" s="9" t="s">
         <v>17</v>
@@ -2723,13 +2810,13 @@
       <c r="I73" s="17"/>
       <c r="J73" s="12"/>
     </row>
-    <row r="74" spans="1:10" s="10" customFormat="1" ht="57">
-      <c r="A74" s="25"/>
-      <c r="B74" s="24"/>
-      <c r="C74" s="20"/>
+    <row r="74" spans="1:10" s="10" customFormat="1" ht="60">
+      <c r="A74" s="21"/>
+      <c r="B74" s="22"/>
+      <c r="C74" s="25"/>
       <c r="D74" s="23"/>
       <c r="E74" s="17" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="F74" s="9" t="s">
         <v>17</v>
@@ -2743,17 +2830,21 @@
       <c r="I74" s="17"/>
       <c r="J74" s="12"/>
     </row>
-    <row r="75" spans="1:10" s="10" customFormat="1" ht="71.25">
-      <c r="A75" s="25"/>
-      <c r="B75" s="24"/>
-      <c r="C75" s="20" t="s">
-        <v>111</v>
+    <row r="75" spans="1:10" s="10" customFormat="1" ht="135">
+      <c r="A75" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="B75" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="C75" s="26" t="s">
+        <v>93</v>
       </c>
       <c r="D75" s="23" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
       <c r="E75" s="17" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="F75" s="9" t="s">
         <v>17</v>
@@ -2767,13 +2858,13 @@
       <c r="I75" s="17"/>
       <c r="J75" s="12"/>
     </row>
-    <row r="76" spans="1:10" s="10" customFormat="1" ht="71.25">
-      <c r="A76" s="25"/>
-      <c r="B76" s="24"/>
-      <c r="C76" s="20"/>
+    <row r="76" spans="1:10" s="10" customFormat="1" ht="75">
+      <c r="A76" s="21"/>
+      <c r="B76" s="22"/>
+      <c r="C76" s="26"/>
       <c r="D76" s="23"/>
       <c r="E76" s="17" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
       <c r="F76" s="9" t="s">
         <v>17</v>
@@ -2787,13 +2878,13 @@
       <c r="I76" s="17"/>
       <c r="J76" s="12"/>
     </row>
-    <row r="77" spans="1:10" s="10" customFormat="1" ht="57">
-      <c r="A77" s="25"/>
-      <c r="B77" s="24"/>
-      <c r="C77" s="20"/>
+    <row r="77" spans="1:10" s="10" customFormat="1" ht="60">
+      <c r="A77" s="21"/>
+      <c r="B77" s="22"/>
+      <c r="C77" s="26"/>
       <c r="D77" s="23"/>
       <c r="E77" s="17" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="F77" s="9" t="s">
         <v>17</v>
@@ -2807,17 +2898,19 @@
       <c r="I77" s="17"/>
       <c r="J77" s="12"/>
     </row>
-    <row r="78" spans="1:10" s="10" customFormat="1" ht="99.75">
-      <c r="A78" s="25"/>
-      <c r="B78" s="24"/>
-      <c r="C78" s="20" t="s">
-        <v>114</v>
+    <row r="78" spans="1:10" s="10" customFormat="1" ht="90">
+      <c r="A78" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="B78" s="22"/>
+      <c r="C78" s="26" t="s">
+        <v>96</v>
       </c>
       <c r="D78" s="23" t="s">
-        <v>115</v>
+        <v>97</v>
       </c>
       <c r="E78" s="17" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="F78" s="9" t="s">
         <v>17</v>
@@ -2831,13 +2924,13 @@
       <c r="I78" s="17"/>
       <c r="J78" s="12"/>
     </row>
-    <row r="79" spans="1:10" s="10" customFormat="1" ht="71.25">
-      <c r="A79" s="25"/>
-      <c r="B79" s="24"/>
-      <c r="C79" s="20"/>
+    <row r="79" spans="1:10" s="10" customFormat="1" ht="75">
+      <c r="A79" s="21"/>
+      <c r="B79" s="22"/>
+      <c r="C79" s="26"/>
       <c r="D79" s="23"/>
       <c r="E79" s="17" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="F79" s="9" t="s">
         <v>17</v>
@@ -2851,13 +2944,13 @@
       <c r="I79" s="17"/>
       <c r="J79" s="12"/>
     </row>
-    <row r="80" spans="1:10" s="10" customFormat="1" ht="57">
-      <c r="A80" s="25"/>
-      <c r="B80" s="24"/>
-      <c r="C80" s="20"/>
+    <row r="80" spans="1:10" s="10" customFormat="1" ht="60">
+      <c r="A80" s="21"/>
+      <c r="B80" s="22"/>
+      <c r="C80" s="26"/>
       <c r="D80" s="23"/>
       <c r="E80" s="17" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="F80" s="9" t="s">
         <v>17</v>
@@ -2871,17 +2964,19 @@
       <c r="I80" s="17"/>
       <c r="J80" s="12"/>
     </row>
-    <row r="81" spans="1:10" s="10" customFormat="1" ht="71.25">
-      <c r="A81" s="25"/>
-      <c r="B81" s="24"/>
+    <row r="81" spans="1:10" s="10" customFormat="1" ht="135">
+      <c r="A81" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="B81" s="22"/>
       <c r="C81" s="26" t="s">
-        <v>116</v>
+        <v>99</v>
       </c>
       <c r="D81" s="23" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="E81" s="17" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="F81" s="9" t="s">
         <v>17</v>
@@ -2895,13 +2990,13 @@
       <c r="I81" s="17"/>
       <c r="J81" s="12"/>
     </row>
-    <row r="82" spans="1:10" s="10" customFormat="1" ht="71.25">
-      <c r="A82" s="25"/>
-      <c r="B82" s="24"/>
+    <row r="82" spans="1:10" s="10" customFormat="1" ht="75">
+      <c r="A82" s="21"/>
+      <c r="B82" s="22"/>
       <c r="C82" s="26"/>
       <c r="D82" s="23"/>
       <c r="E82" s="17" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
       <c r="F82" s="9" t="s">
         <v>17</v>
@@ -2915,13 +3010,13 @@
       <c r="I82" s="17"/>
       <c r="J82" s="12"/>
     </row>
-    <row r="83" spans="1:10" s="10" customFormat="1" ht="57">
-      <c r="A83" s="25"/>
-      <c r="B83" s="24"/>
+    <row r="83" spans="1:10" s="10" customFormat="1" ht="60">
+      <c r="A83" s="21"/>
+      <c r="B83" s="22"/>
       <c r="C83" s="26"/>
       <c r="D83" s="23"/>
       <c r="E83" s="17" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="F83" s="9" t="s">
         <v>17</v>
@@ -2935,17 +3030,19 @@
       <c r="I83" s="17"/>
       <c r="J83" s="12"/>
     </row>
-    <row r="84" spans="1:10" s="10" customFormat="1" ht="99.75">
-      <c r="A84" s="25"/>
-      <c r="B84" s="24"/>
-      <c r="C84" s="26" t="s">
-        <v>118</v>
+    <row r="84" spans="1:10" s="10" customFormat="1" ht="90">
+      <c r="A84" s="21" t="s">
+        <v>140</v>
+      </c>
+      <c r="B84" s="22"/>
+      <c r="C84" s="25" t="s">
+        <v>101</v>
       </c>
       <c r="D84" s="23" t="s">
-        <v>119</v>
+        <v>102</v>
       </c>
       <c r="E84" s="17" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="F84" s="9" t="s">
         <v>17</v>
@@ -2959,13 +3056,13 @@
       <c r="I84" s="17"/>
       <c r="J84" s="12"/>
     </row>
-    <row r="85" spans="1:10" s="10" customFormat="1" ht="71.25">
-      <c r="A85" s="25"/>
-      <c r="B85" s="24"/>
-      <c r="C85" s="26"/>
+    <row r="85" spans="1:10" s="10" customFormat="1" ht="75">
+      <c r="A85" s="21"/>
+      <c r="B85" s="22"/>
+      <c r="C85" s="25"/>
       <c r="D85" s="23"/>
       <c r="E85" s="17" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="F85" s="9" t="s">
         <v>17</v>
@@ -2979,13 +3076,13 @@
       <c r="I85" s="17"/>
       <c r="J85" s="12"/>
     </row>
-    <row r="86" spans="1:10" s="10" customFormat="1" ht="57">
-      <c r="A86" s="25"/>
-      <c r="B86" s="24"/>
-      <c r="C86" s="26"/>
+    <row r="86" spans="1:10" s="10" customFormat="1" ht="60">
+      <c r="A86" s="21"/>
+      <c r="B86" s="22"/>
+      <c r="C86" s="25"/>
       <c r="D86" s="23"/>
       <c r="E86" s="17" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="F86" s="9" t="s">
         <v>17</v>
@@ -2999,17 +3096,19 @@
       <c r="I86" s="17"/>
       <c r="J86" s="12"/>
     </row>
-    <row r="87" spans="1:10" s="10" customFormat="1" ht="71.25">
-      <c r="A87" s="25"/>
-      <c r="B87" s="24"/>
-      <c r="C87" s="26" t="s">
-        <v>121</v>
+    <row r="87" spans="1:10" s="10" customFormat="1" ht="135">
+      <c r="A87" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="B87" s="22"/>
+      <c r="C87" s="25" t="s">
+        <v>103</v>
       </c>
       <c r="D87" s="23" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="E87" s="17" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="F87" s="9" t="s">
         <v>17</v>
@@ -3023,13 +3122,13 @@
       <c r="I87" s="17"/>
       <c r="J87" s="12"/>
     </row>
-    <row r="88" spans="1:10" s="10" customFormat="1" ht="71.25">
-      <c r="A88" s="25"/>
-      <c r="B88" s="24"/>
-      <c r="C88" s="26"/>
+    <row r="88" spans="1:10" s="10" customFormat="1" ht="75">
+      <c r="A88" s="21"/>
+      <c r="B88" s="22"/>
+      <c r="C88" s="25"/>
       <c r="D88" s="23"/>
       <c r="E88" s="17" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
       <c r="F88" s="9" t="s">
         <v>17</v>
@@ -3043,13 +3142,13 @@
       <c r="I88" s="17"/>
       <c r="J88" s="12"/>
     </row>
-    <row r="89" spans="1:10" s="10" customFormat="1" ht="57">
-      <c r="A89" s="25"/>
-      <c r="B89" s="24"/>
-      <c r="C89" s="26"/>
+    <row r="89" spans="1:10" s="10" customFormat="1" ht="60">
+      <c r="A89" s="21"/>
+      <c r="B89" s="22"/>
+      <c r="C89" s="25"/>
       <c r="D89" s="23"/>
       <c r="E89" s="17" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="F89" s="9" t="s">
         <v>17</v>
@@ -3063,17 +3162,19 @@
       <c r="I89" s="17"/>
       <c r="J89" s="12"/>
     </row>
-    <row r="90" spans="1:10" s="10" customFormat="1" ht="99.75">
-      <c r="A90" s="25"/>
-      <c r="B90" s="24"/>
-      <c r="C90" s="22" t="s">
-        <v>122</v>
+    <row r="90" spans="1:10" s="10" customFormat="1" ht="90">
+      <c r="A90" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="B90" s="22"/>
+      <c r="C90" s="25" t="s">
+        <v>106</v>
       </c>
       <c r="D90" s="23" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="E90" s="17" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="F90" s="9" t="s">
         <v>17</v>
@@ -3087,13 +3188,13 @@
       <c r="I90" s="17"/>
       <c r="J90" s="12"/>
     </row>
-    <row r="91" spans="1:10" s="10" customFormat="1" ht="71.25">
-      <c r="A91" s="25"/>
-      <c r="B91" s="24"/>
-      <c r="C91" s="22"/>
+    <row r="91" spans="1:10" s="10" customFormat="1" ht="75">
+      <c r="A91" s="21"/>
+      <c r="B91" s="22"/>
+      <c r="C91" s="25"/>
       <c r="D91" s="23"/>
       <c r="E91" s="17" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="F91" s="9" t="s">
         <v>17</v>
@@ -3107,13 +3208,13 @@
       <c r="I91" s="17"/>
       <c r="J91" s="12"/>
     </row>
-    <row r="92" spans="1:10" s="10" customFormat="1" ht="57">
-      <c r="A92" s="25"/>
-      <c r="B92" s="24"/>
-      <c r="C92" s="22"/>
+    <row r="92" spans="1:10" s="10" customFormat="1" ht="60">
+      <c r="A92" s="21"/>
+      <c r="B92" s="22"/>
+      <c r="C92" s="25"/>
       <c r="D92" s="23"/>
       <c r="E92" s="17" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="F92" s="9" t="s">
         <v>17</v>
@@ -3127,17 +3228,19 @@
       <c r="I92" s="17"/>
       <c r="J92" s="12"/>
     </row>
-    <row r="93" spans="1:10" s="10" customFormat="1" ht="71.25">
-      <c r="A93" s="25"/>
-      <c r="B93" s="24"/>
-      <c r="C93" s="22" t="s">
-        <v>123</v>
+    <row r="93" spans="1:10" s="10" customFormat="1" ht="135">
+      <c r="A93" s="21" t="s">
+        <v>143</v>
+      </c>
+      <c r="B93" s="22"/>
+      <c r="C93" s="26" t="s">
+        <v>107</v>
       </c>
       <c r="D93" s="23" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="E93" s="17" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="F93" s="9" t="s">
         <v>17</v>
@@ -3151,13 +3254,13 @@
       <c r="I93" s="17"/>
       <c r="J93" s="12"/>
     </row>
-    <row r="94" spans="1:10" s="10" customFormat="1" ht="71.25">
-      <c r="A94" s="25"/>
-      <c r="B94" s="24"/>
-      <c r="C94" s="22"/>
+    <row r="94" spans="1:10" s="10" customFormat="1" ht="75">
+      <c r="A94" s="21"/>
+      <c r="B94" s="22"/>
+      <c r="C94" s="26"/>
       <c r="D94" s="23"/>
       <c r="E94" s="17" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
       <c r="F94" s="9" t="s">
         <v>17</v>
@@ -3171,13 +3274,13 @@
       <c r="I94" s="17"/>
       <c r="J94" s="12"/>
     </row>
-    <row r="95" spans="1:10" s="10" customFormat="1" ht="57">
-      <c r="A95" s="25"/>
-      <c r="B95" s="24"/>
-      <c r="C95" s="22"/>
+    <row r="95" spans="1:10" s="10" customFormat="1" ht="60">
+      <c r="A95" s="21"/>
+      <c r="B95" s="22"/>
+      <c r="C95" s="26"/>
       <c r="D95" s="23"/>
       <c r="E95" s="17" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="F95" s="9" t="s">
         <v>17</v>
@@ -3191,75 +3294,140 @@
       <c r="I95" s="17"/>
       <c r="J95" s="12"/>
     </row>
-    <row r="96" spans="1:10" s="10" customFormat="1">
-      <c r="A96" s="18"/>
-      <c r="B96" s="19"/>
-      <c r="C96"/>
-      <c r="D96" s="21"/>
-      <c r="E96" s="17"/>
-      <c r="F96" s="9"/>
-      <c r="G96" s="17"/>
-      <c r="H96" s="9"/>
+    <row r="96" spans="1:10" s="10" customFormat="1" ht="90">
+      <c r="A96" s="21" t="s">
+        <v>144</v>
+      </c>
+      <c r="B96" s="22"/>
+      <c r="C96" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="D96" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="E96" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="F96" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G96" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="H96" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="I96" s="17"/>
       <c r="J96" s="12"/>
     </row>
-    <row r="97" spans="1:10" s="13" customFormat="1">
-      <c r="A97" s="27" t="s">
+    <row r="97" spans="1:10" s="10" customFormat="1" ht="75">
+      <c r="A97" s="21"/>
+      <c r="B97" s="22"/>
+      <c r="C97" s="26"/>
+      <c r="D97" s="23"/>
+      <c r="E97" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="F97" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G97" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="H97" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I97" s="17"/>
+      <c r="J97" s="12"/>
+    </row>
+    <row r="98" spans="1:10" s="10" customFormat="1" ht="60">
+      <c r="A98" s="21"/>
+      <c r="B98" s="22"/>
+      <c r="C98" s="26"/>
+      <c r="D98" s="23"/>
+      <c r="E98" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="F98" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G98" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="H98" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I98" s="17"/>
+      <c r="J98" s="12"/>
+    </row>
+    <row r="99" spans="1:10" s="10" customFormat="1">
+      <c r="A99" s="18"/>
+      <c r="B99" s="19"/>
+      <c r="C99"/>
+      <c r="D99" s="20"/>
+      <c r="E99" s="17"/>
+      <c r="F99" s="9"/>
+      <c r="G99" s="17"/>
+      <c r="H99" s="9"/>
+      <c r="I99" s="17"/>
+      <c r="J99" s="12"/>
+    </row>
+    <row r="100" spans="1:10" s="13" customFormat="1">
+      <c r="A100" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="B97" s="27"/>
-      <c r="C97" s="27"/>
-      <c r="D97" s="27"/>
-      <c r="E97" s="27"/>
-      <c r="F97" s="27"/>
-      <c r="G97" s="27"/>
-      <c r="H97" s="27"/>
-      <c r="I97" s="27"/>
-      <c r="J97" s="27"/>
+      <c r="B100" s="24"/>
+      <c r="C100" s="24"/>
+      <c r="D100" s="24"/>
+      <c r="E100" s="24"/>
+      <c r="F100" s="24"/>
+      <c r="G100" s="24"/>
+      <c r="H100" s="24"/>
+      <c r="I100" s="24"/>
+      <c r="J100" s="24"/>
     </row>
   </sheetData>
-  <mergeCells count="73">
-    <mergeCell ref="A60:A62"/>
-    <mergeCell ref="B12:B62"/>
-    <mergeCell ref="A57:A59"/>
+  <mergeCells count="95">
     <mergeCell ref="D63:D65"/>
-    <mergeCell ref="D57:D59"/>
-    <mergeCell ref="C57:C59"/>
-    <mergeCell ref="D60:D62"/>
-    <mergeCell ref="C60:C62"/>
-    <mergeCell ref="D48:D50"/>
-    <mergeCell ref="D51:D53"/>
-    <mergeCell ref="D54:D56"/>
-    <mergeCell ref="A48:A56"/>
-    <mergeCell ref="C48:C50"/>
-    <mergeCell ref="C51:C53"/>
-    <mergeCell ref="C54:C56"/>
-    <mergeCell ref="C42:C44"/>
-    <mergeCell ref="D42:D44"/>
-    <mergeCell ref="D45:D47"/>
-    <mergeCell ref="A39:A47"/>
-    <mergeCell ref="C45:C47"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="A21:A32"/>
-    <mergeCell ref="A33:A38"/>
-    <mergeCell ref="D39:D41"/>
-    <mergeCell ref="C39:C41"/>
-    <mergeCell ref="A3:A11"/>
-    <mergeCell ref="B3:B11"/>
-    <mergeCell ref="C27:C29"/>
-    <mergeCell ref="D27:D29"/>
-    <mergeCell ref="D30:D32"/>
-    <mergeCell ref="C30:C32"/>
-    <mergeCell ref="D33:D35"/>
-    <mergeCell ref="C33:C35"/>
-    <mergeCell ref="D36:D38"/>
-    <mergeCell ref="C36:C38"/>
-    <mergeCell ref="D6:D8"/>
-    <mergeCell ref="C6:C8"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="A12:A17"/>
-    <mergeCell ref="A97:J97"/>
+    <mergeCell ref="A96:A98"/>
+    <mergeCell ref="A63:A65"/>
+    <mergeCell ref="B12:B65"/>
+    <mergeCell ref="A69:A71"/>
+    <mergeCell ref="A72:A74"/>
+    <mergeCell ref="A75:A77"/>
+    <mergeCell ref="A78:A80"/>
+    <mergeCell ref="A81:A83"/>
+    <mergeCell ref="A45:A47"/>
+    <mergeCell ref="A48:A50"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A54:A56"/>
+    <mergeCell ref="A66:A68"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="A42:A44"/>
+    <mergeCell ref="D93:D95"/>
+    <mergeCell ref="D96:D98"/>
+    <mergeCell ref="B75:B98"/>
+    <mergeCell ref="D87:D89"/>
+    <mergeCell ref="D90:D92"/>
+    <mergeCell ref="C90:C92"/>
+    <mergeCell ref="C87:C89"/>
+    <mergeCell ref="D78:D80"/>
+    <mergeCell ref="D81:D83"/>
+    <mergeCell ref="C84:C86"/>
+    <mergeCell ref="D84:D86"/>
+    <mergeCell ref="A84:A86"/>
+    <mergeCell ref="A87:A89"/>
+    <mergeCell ref="A90:A92"/>
+    <mergeCell ref="A93:A95"/>
+    <mergeCell ref="C69:C71"/>
+    <mergeCell ref="C72:C74"/>
+    <mergeCell ref="C66:C68"/>
+    <mergeCell ref="D75:D77"/>
+    <mergeCell ref="D69:D71"/>
+    <mergeCell ref="A100:J100"/>
     <mergeCell ref="C3:C5"/>
     <mergeCell ref="D3:D5"/>
     <mergeCell ref="D12:D14"/>
@@ -3272,26 +3440,49 @@
     <mergeCell ref="D21:D23"/>
     <mergeCell ref="C24:C26"/>
     <mergeCell ref="D24:D26"/>
-    <mergeCell ref="D69:D71"/>
-    <mergeCell ref="B63:B71"/>
-    <mergeCell ref="A63:A71"/>
-    <mergeCell ref="C66:C68"/>
-    <mergeCell ref="C69:C71"/>
-    <mergeCell ref="C63:C65"/>
     <mergeCell ref="D72:D74"/>
+    <mergeCell ref="B66:B74"/>
+    <mergeCell ref="B3:B11"/>
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="D27:D29"/>
+    <mergeCell ref="D30:D32"/>
+    <mergeCell ref="C30:C32"/>
+    <mergeCell ref="D6:D8"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="D42:D44"/>
+    <mergeCell ref="D45:D47"/>
+    <mergeCell ref="C45:C47"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="D39:D41"/>
+    <mergeCell ref="C39:C41"/>
+    <mergeCell ref="D33:D35"/>
+    <mergeCell ref="C33:C35"/>
+    <mergeCell ref="D36:D38"/>
+    <mergeCell ref="C36:C38"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="A60:A62"/>
+    <mergeCell ref="A57:A59"/>
     <mergeCell ref="D66:D68"/>
-    <mergeCell ref="D90:D92"/>
-    <mergeCell ref="D93:D95"/>
-    <mergeCell ref="B72:B95"/>
-    <mergeCell ref="A72:A95"/>
-    <mergeCell ref="D84:D86"/>
-    <mergeCell ref="D87:D89"/>
-    <mergeCell ref="C87:C89"/>
-    <mergeCell ref="C84:C86"/>
-    <mergeCell ref="D75:D77"/>
-    <mergeCell ref="D78:D80"/>
-    <mergeCell ref="C81:C83"/>
-    <mergeCell ref="D81:D83"/>
+    <mergeCell ref="D57:D59"/>
+    <mergeCell ref="C57:C59"/>
+    <mergeCell ref="D60:D62"/>
+    <mergeCell ref="C60:C62"/>
+    <mergeCell ref="D48:D50"/>
+    <mergeCell ref="D51:D53"/>
+    <mergeCell ref="D54:D56"/>
+    <mergeCell ref="C48:C50"/>
+    <mergeCell ref="C51:C53"/>
+    <mergeCell ref="C54:C56"/>
+    <mergeCell ref="C42:C44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3302,19 +3493,19 @@
           <x14:formula1>
             <xm:f>DONOTDELETE!$A$3:$A$10</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F96</xm:sqref>
+          <xm:sqref>F2:F99</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A82C53B1-967F-492E-998A-B9F5A535C02B}">
           <x14:formula1>
             <xm:f>DONOTDELETE!$C$3:$C$10</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G96</xm:sqref>
+          <xm:sqref>G2:G99</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{AA44578F-B7B1-435C-B81D-7B38EFD8E099}">
           <x14:formula1>
             <xm:f>DONOTDELETE!$E$3:$E$7</xm:f>
           </x14:formula1>
-          <xm:sqref>H2:H96</xm:sqref>
+          <xm:sqref>H2:H99</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>